<commit_message>
Correccion del nombre de un integrante
Se modifico el dato de un integrante
</commit_message>
<xml_diff>
--- a/documentos/Plantilla de Product Backlog.xlsx
+++ b/documentos/Plantilla de Product Backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TP Inge 2\IS2\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -280,13 +280,13 @@
     <t>crear flujos Kanban</t>
   </si>
   <si>
-    <t>Elaborado por:  Jacqueline Gill, Pablo Aguilar, Porfirio Pérez y Óscar Vega</t>
+    <t>Elaborado por:  Jacqueline Gill, Pablo Aguilar, Porfirio Pérez y Oscar Vega</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -746,14 +746,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>11</v>
       </c>
@@ -1315,14 +1315,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="5" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="5" customWidth="1"/>

</xml_diff>